<commit_message>
pending list, rejected list, approved list (theses)
</commit_message>
<xml_diff>
--- a/Source/GraduateThesisManagement/GraduateThesis.Web/wwwroot/reports/rejected-thesis_export.xlsx
+++ b/Source/GraduateThesisManagement/GraduateThesis.Web/wwwroot/reports/rejected-thesis_export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HUFI_GRADUATE-THESIS\HUFI_graduate-thesis-management\Source\GraduateThesisManagement\GraduateThesis.Web\wwwroot\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6C2D1F-E051-4361-B6EB-77AFE19B2362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7819DD69-A9A0-4AE7-B432-F327BE0B0A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9618D36F-91D3-4472-B248-079CF11FD3FC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>STT</t>
   </si>
@@ -50,9 +50,6 @@
     <t>{{Items.Name}}</t>
   </si>
   <si>
-    <t>DANH SÁCH ĐỀ TÀI KHÓA LUẬN CỦA KHOA CÔNG NGHỆ THÔNG TIN</t>
-  </si>
-  <si>
     <t>Mã đề tài</t>
   </si>
   <si>
@@ -93,6 +90,15 @@
   </si>
   <si>
     <t>{{Items.TopicName}}</t>
+  </si>
+  <si>
+    <t>{{Name}}</t>
+  </si>
+  <si>
+    <t>Lý do từ chối</t>
+  </si>
+  <si>
+    <t>{{Items.Notes}}</t>
   </si>
 </sst>
 </file>
@@ -196,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -209,9 +215,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21335E7-9D2F-4669-9087-ECB332918034}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -549,85 +552,93 @@
     <col min="7" max="7" width="20.21875" customWidth="1"/>
     <col min="8" max="8" width="23.77734375" customWidth="1"/>
     <col min="9" max="9" width="29.21875" customWidth="1"/>
+    <col min="10" max="10" width="47.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.6" customHeight="1" thickBot="1">
-      <c r="A1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+    <row r="1" spans="1:10" ht="33.6" customHeight="1" thickBot="1">
+      <c r="A1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="22.2" customHeight="1" thickBot="1">
+    <row r="2" spans="1:10" ht="22.2" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.4" customHeight="1">
+    <row r="3" spans="1:10" ht="38.4" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>15</v>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="C6" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>